<commit_message>
excel data changed -> 96 scenarios in total
</commit_message>
<xml_diff>
--- a/data/input_investment/InvestmentScenario_OperationEnergyCost.xlsx
+++ b/data/input_investment/InvestmentScenario_OperationEnergyCost.xlsx
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>91232.32623729082</v>
+        <v>120716.1522112524</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>112672.8495605371</v>
+        <v>139051.7984401947</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>93437.5379989362</v>
+        <v>122584.2638928925</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>117300.523453884</v>
+        <v>143467.8780872832</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -894,7 +894,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>92972.38984089519</v>
+        <v>121897.7867472824</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -941,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>114992.4748169564</v>
+        <v>141028.3171938551</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -1082,7 +1082,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>95657.22597281073</v>
+        <v>124177.2568180901</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -1129,7 +1129,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>120199.8818108463</v>
+        <v>145824.7654788709</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -1270,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>121618.9847831144</v>
+        <v>142022.830156972</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -1317,7 +1317,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>153491.755558488</v>
+        <v>170923.5954583264</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -1458,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>121485.6425153304</v>
+        <v>141864.4580373701</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -1505,7 +1505,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>153363.1531495027</v>
+        <v>170794.4238972236</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -1646,7 +1646,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>121496.2419411142</v>
+        <v>141874.069189175</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -1693,7 +1693,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>153373.2064023471</v>
+        <v>170804.409701393</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -1834,7 +1834,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>121363.7340781308</v>
+        <v>141715.9680147173</v>
       </c>
       <c r="D30" t="n">
         <v>1</v>
@@ -1881,7 +1881,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>153244.7366927499</v>
+        <v>170675.3451249267</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
@@ -2022,7 +2022,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>151404.5089722227</v>
+        <v>184772.8045993561</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -2069,7 +2069,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>170033.3769332291</v>
+        <v>200441.6653923719</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -2210,7 +2210,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>153349.2011734893</v>
+        <v>186148.520469406</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
@@ -2257,7 +2257,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>174382.5103821395</v>
+        <v>204072.0946239115</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -2398,7 +2398,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>153925.491105069</v>
+        <v>186036.1053038605</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -2445,7 +2445,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>173922.3290696569</v>
+        <v>202931.8747747873</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -2586,7 +2586,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>156422.3771281044</v>
+        <v>187927.231350612</v>
       </c>
       <c r="D46" t="n">
         <v>1</v>
@@ -2633,7 +2633,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>178844.8168405278</v>
+        <v>207255.2241745333</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
@@ -2774,7 +2774,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>186807.6023249842</v>
+        <v>207211.4476988417</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
@@ -2821,7 +2821,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>218714.9069322415</v>
+        <v>236146.7467773402</v>
       </c>
       <c r="D51" t="n">
         <v>1</v>
@@ -2962,7 +2962,7 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>186674.2600511219</v>
+        <v>207053.0755731615</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
@@ -3009,7 +3009,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>218586.3046932528</v>
+        <v>236017.5756465657</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
@@ -3150,7 +3150,7 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>186684.8594799448</v>
+        <v>207062.6867280056</v>
       </c>
       <c r="D58" t="n">
         <v>1</v>
@@ -3197,7 +3197,7 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>218596.3579430582</v>
+        <v>236027.5612394723</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -3338,7 +3338,7 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>186552.3516169615</v>
+        <v>206904.5855535479</v>
       </c>
       <c r="D62" t="n">
         <v>1</v>
@@ -3385,7 +3385,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>218467.8882334609</v>
+        <v>235898.4966656377</v>
       </c>
       <c r="D63" t="n">
         <v>1</v>
@@ -3526,7 +3526,7 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>199650.1093002641</v>
+        <v>234906.859567781</v>
       </c>
       <c r="D66" t="n">
         <v>1</v>
@@ -3573,7 +3573,7 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>216837.1863967776</v>
+        <v>249470.2379004707</v>
       </c>
       <c r="D67" t="n">
         <v>1</v>
@@ -3714,7 +3714,7 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>201462.3056847866</v>
+        <v>236064.9238989371</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
@@ -3761,7 +3761,7 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>221018.0173779749</v>
+        <v>252786.2787378968</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -3902,7 +3902,7 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>202904.8943058239</v>
+        <v>236635.6795396588</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -3949,7 +3949,7 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>222228.5484548758</v>
+        <v>252773.824457818</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
@@ -4090,7 +4090,7 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>205445.6216179376</v>
+        <v>238447.614645082</v>
       </c>
       <c r="D78" t="n">
         <v>1</v>
@@ -4137,7 +4137,7 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>227136.2092227579</v>
+        <v>256959.3831505053</v>
       </c>
       <c r="D79" t="n">
         <v>1</v>
@@ -4278,7 +4278,7 @@
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>240369.9672584436</v>
+        <v>260773.8126323012</v>
       </c>
       <c r="D82" t="n">
         <v>1</v>
@@ -4325,7 +4325,7 @@
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>272287.0848770291</v>
+        <v>289718.9247643672</v>
       </c>
       <c r="D83" t="n">
         <v>1</v>
@@ -4466,7 +4466,7 @@
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>240236.6249906596</v>
+        <v>260615.4405126992</v>
       </c>
       <c r="D86" t="n">
         <v>1</v>
@@ -4513,7 +4513,7 @@
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>272158.4824585827</v>
+        <v>289589.7534118955</v>
       </c>
       <c r="D87" t="n">
         <v>1</v>
@@ -4654,7 +4654,7 @@
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>240247.2244164434</v>
+        <v>260625.0516645042</v>
       </c>
       <c r="D90" t="n">
         <v>1</v>
@@ -4701,7 +4701,7 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>272168.535708388</v>
+        <v>289599.7390148292</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
@@ -4842,7 +4842,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>240114.71655346</v>
+        <v>260466.9504900465</v>
       </c>
       <c r="D94" t="n">
         <v>1</v>
@@ -4889,7 +4889,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="n">
-        <v>272040.0659987908</v>
+        <v>289470.6744309675</v>
       </c>
       <c r="D95" t="n">
         <v>1</v>
@@ -5030,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="C98" t="n">
-        <v>98977.83179601947</v>
+        <v>125819.7983852314</v>
       </c>
       <c r="D98" t="n">
         <v>2</v>
@@ -5077,7 +5077,7 @@
         <v>2</v>
       </c>
       <c r="C99" t="n">
-        <v>129565.4283934312</v>
+        <v>152295.34210942</v>
       </c>
       <c r="D99" t="n">
         <v>2</v>
@@ -5218,7 +5218,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="n">
-        <v>106333.5935703312</v>
+        <v>131660.3520990623</v>
       </c>
       <c r="D102" t="n">
         <v>2</v>
@@ -5265,7 +5265,7 @@
         <v>6</v>
       </c>
       <c r="C103" t="n">
-        <v>137163.717426875</v>
+        <v>158685.4376367659</v>
       </c>
       <c r="D103" t="n">
         <v>2</v>
@@ -5406,7 +5406,7 @@
         <v>9</v>
       </c>
       <c r="C106" t="n">
-        <v>98977.83179601947</v>
+        <v>125819.7983852314</v>
       </c>
       <c r="D106" t="n">
         <v>2</v>
@@ -5453,7 +5453,7 @@
         <v>10</v>
       </c>
       <c r="C107" t="n">
-        <v>129565.4283934312</v>
+        <v>152295.34210942</v>
       </c>
       <c r="D107" t="n">
         <v>2</v>
@@ -5594,7 +5594,7 @@
         <v>13</v>
       </c>
       <c r="C110" t="n">
-        <v>106333.5935703312</v>
+        <v>131660.3520990623</v>
       </c>
       <c r="D110" t="n">
         <v>2</v>
@@ -5641,7 +5641,7 @@
         <v>14</v>
       </c>
       <c r="C111" t="n">
-        <v>137163.717426875</v>
+        <v>158685.4376367659</v>
       </c>
       <c r="D111" t="n">
         <v>2</v>
@@ -5782,7 +5782,7 @@
         <v>17</v>
       </c>
       <c r="C114" t="n">
-        <v>122249.7460384077</v>
+        <v>142591.0276293001</v>
       </c>
       <c r="D114" t="n">
         <v>2</v>
@@ -5829,7 +5829,7 @@
         <v>18</v>
       </c>
       <c r="C115" t="n">
-        <v>154092.0632758084</v>
+        <v>171514.5651693879</v>
       </c>
       <c r="D115" t="n">
         <v>2</v>
@@ -5970,7 +5970,7 @@
         <v>21</v>
       </c>
       <c r="C118" t="n">
-        <v>121455.0694251249</v>
+        <v>141799.4095141054</v>
       </c>
       <c r="D118" t="n">
         <v>2</v>
@@ -6017,7 +6017,7 @@
         <v>22</v>
       </c>
       <c r="C119" t="n">
-        <v>153244.7366927499</v>
+        <v>170675.3451249266</v>
       </c>
       <c r="D119" t="n">
         <v>2</v>
@@ -6158,7 +6158,7 @@
         <v>25</v>
       </c>
       <c r="C122" t="n">
-        <v>122249.7460384077</v>
+        <v>142591.0276293001</v>
       </c>
       <c r="D122" t="n">
         <v>2</v>
@@ -6205,7 +6205,7 @@
         <v>26</v>
       </c>
       <c r="C123" t="n">
-        <v>154092.0632758084</v>
+        <v>171514.5651693879</v>
       </c>
       <c r="D123" t="n">
         <v>2</v>
@@ -6346,7 +6346,7 @@
         <v>29</v>
       </c>
       <c r="C126" t="n">
-        <v>121455.0694251249</v>
+        <v>141799.4095141054</v>
       </c>
       <c r="D126" t="n">
         <v>2</v>
@@ -6393,7 +6393,7 @@
         <v>30</v>
       </c>
       <c r="C127" t="n">
-        <v>153244.7366927499</v>
+        <v>170675.3451249266</v>
       </c>
       <c r="D127" t="n">
         <v>2</v>
@@ -6534,7 +6534,7 @@
         <v>33</v>
       </c>
       <c r="C130" t="n">
-        <v>161636.8512419319</v>
+        <v>190229.2404402616</v>
       </c>
       <c r="D130" t="n">
         <v>2</v>
@@ -6581,7 +6581,7 @@
         <v>34</v>
       </c>
       <c r="C131" t="n">
-        <v>189192.4179039672</v>
+        <v>214131.6591120306</v>
       </c>
       <c r="D131" t="n">
         <v>2</v>
@@ -6722,7 +6722,7 @@
         <v>37</v>
       </c>
       <c r="C134" t="n">
-        <v>167960.0510283367</v>
+        <v>195648.0359737862</v>
       </c>
       <c r="D134" t="n">
         <v>2</v>
@@ -6769,7 +6769,7 @@
         <v>38</v>
       </c>
       <c r="C135" t="n">
-        <v>195911.5085041784</v>
+        <v>219586.4475331511</v>
       </c>
       <c r="D135" t="n">
         <v>2</v>
@@ -6910,7 +6910,7 @@
         <v>41</v>
       </c>
       <c r="C138" t="n">
-        <v>161636.8512419319</v>
+        <v>190229.2404402616</v>
       </c>
       <c r="D138" t="n">
         <v>2</v>
@@ -6957,7 +6957,7 @@
         <v>42</v>
       </c>
       <c r="C139" t="n">
-        <v>189192.4179039672</v>
+        <v>214131.6591120306</v>
       </c>
       <c r="D139" t="n">
         <v>2</v>
@@ -7098,7 +7098,7 @@
         <v>45</v>
       </c>
       <c r="C142" t="n">
-        <v>167960.0510283367</v>
+        <v>195648.0359737862</v>
       </c>
       <c r="D142" t="n">
         <v>2</v>
@@ -7145,7 +7145,7 @@
         <v>46</v>
       </c>
       <c r="C143" t="n">
-        <v>195911.5085041784</v>
+        <v>219586.4475331511</v>
       </c>
       <c r="D143" t="n">
         <v>2</v>
@@ -7286,7 +7286,7 @@
         <v>49</v>
       </c>
       <c r="C146" t="n">
-        <v>187472.8975791187</v>
+        <v>207814.1791700112</v>
       </c>
       <c r="D146" t="n">
         <v>2</v>
@@ -7333,7 +7333,7 @@
         <v>50</v>
       </c>
       <c r="C147" t="n">
-        <v>219315.2148165194</v>
+        <v>236737.716710099</v>
       </c>
       <c r="D147" t="n">
         <v>2</v>
@@ -7474,7 +7474,7 @@
         <v>53</v>
       </c>
       <c r="C150" t="n">
-        <v>186678.2209658359</v>
+        <v>207022.5610548165</v>
       </c>
       <c r="D150" t="n">
         <v>2</v>
@@ -7521,7 +7521,7 @@
         <v>54</v>
       </c>
       <c r="C151" t="n">
-        <v>218467.8882334609</v>
+        <v>235898.4966656376</v>
       </c>
       <c r="D151" t="n">
         <v>2</v>
@@ -7662,7 +7662,7 @@
         <v>57</v>
       </c>
       <c r="C154" t="n">
-        <v>187472.8975791187</v>
+        <v>207814.1791700112</v>
       </c>
       <c r="D154" t="n">
         <v>2</v>
@@ -7709,7 +7709,7 @@
         <v>58</v>
       </c>
       <c r="C155" t="n">
-        <v>219315.2148165194</v>
+        <v>236737.716710099</v>
       </c>
       <c r="D155" t="n">
         <v>2</v>
@@ -7850,7 +7850,7 @@
         <v>61</v>
       </c>
       <c r="C158" t="n">
-        <v>186678.2209658359</v>
+        <v>207022.5610548165</v>
       </c>
       <c r="D158" t="n">
         <v>2</v>
@@ -7897,7 +7897,7 @@
         <v>62</v>
       </c>
       <c r="C159" t="n">
-        <v>218467.8882334609</v>
+        <v>235898.4966656376</v>
       </c>
       <c r="D159" t="n">
         <v>2</v>
@@ -8038,7 +8038,7 @@
         <v>65</v>
       </c>
       <c r="C162" t="n">
-        <v>210520.0964374705</v>
+        <v>240340.4944477063</v>
       </c>
       <c r="D162" t="n">
         <v>2</v>
@@ -8085,7 +8085,7 @@
         <v>66</v>
       </c>
       <c r="C163" t="n">
-        <v>236820.4458745822</v>
+        <v>263076.5815397532</v>
       </c>
       <c r="D163" t="n">
         <v>2</v>
@@ -8226,7 +8226,7 @@
         <v>69</v>
       </c>
       <c r="C166" t="n">
-        <v>216402.810551186</v>
+        <v>245577.5501851852</v>
       </c>
       <c r="D166" t="n">
         <v>2</v>
@@ -8273,7 +8273,7 @@
         <v>70</v>
       </c>
       <c r="C167" t="n">
-        <v>242881.6645736336</v>
+        <v>268186.0062417226</v>
       </c>
       <c r="D167" t="n">
         <v>2</v>
@@ -8414,7 +8414,7 @@
         <v>73</v>
       </c>
       <c r="C170" t="n">
-        <v>210520.0964374705</v>
+        <v>240340.4944477063</v>
       </c>
       <c r="D170" t="n">
         <v>2</v>
@@ -8461,7 +8461,7 @@
         <v>74</v>
       </c>
       <c r="C171" t="n">
-        <v>236820.4458745822</v>
+        <v>263076.5815397532</v>
       </c>
       <c r="D171" t="n">
         <v>2</v>
@@ -8602,7 +8602,7 @@
         <v>77</v>
       </c>
       <c r="C174" t="n">
-        <v>216402.810551186</v>
+        <v>245577.5501851852</v>
       </c>
       <c r="D174" t="n">
         <v>2</v>
@@ -8649,7 +8649,7 @@
         <v>78</v>
       </c>
       <c r="C175" t="n">
-        <v>242881.6645736336</v>
+        <v>268186.0062417226</v>
       </c>
       <c r="D175" t="n">
         <v>2</v>
@@ -8790,7 +8790,7 @@
         <v>81</v>
       </c>
       <c r="C178" t="n">
-        <v>241045.0753444486</v>
+        <v>261386.356935341</v>
       </c>
       <c r="D178" t="n">
         <v>2</v>
@@ -8837,7 +8837,7 @@
         <v>82</v>
       </c>
       <c r="C179" t="n">
-        <v>272887.3925818492</v>
+        <v>290309.8944754287</v>
       </c>
       <c r="D179" t="n">
         <v>2</v>
@@ -8978,7 +8978,7 @@
         <v>85</v>
       </c>
       <c r="C182" t="n">
-        <v>240250.3987311658</v>
+        <v>260594.7388201463</v>
       </c>
       <c r="D182" t="n">
         <v>2</v>
@@ -9025,7 +9025,7 @@
         <v>86</v>
       </c>
       <c r="C183" t="n">
-        <v>272040.0659987907</v>
+        <v>289470.6744309674</v>
       </c>
       <c r="D183" t="n">
         <v>2</v>
@@ -9166,7 +9166,7 @@
         <v>89</v>
       </c>
       <c r="C186" t="n">
-        <v>241045.0753444486</v>
+        <v>261386.356935341</v>
       </c>
       <c r="D186" t="n">
         <v>2</v>
@@ -9213,7 +9213,7 @@
         <v>90</v>
       </c>
       <c r="C187" t="n">
-        <v>272887.3925818492</v>
+        <v>290309.8944754287</v>
       </c>
       <c r="D187" t="n">
         <v>2</v>
@@ -9354,7 +9354,7 @@
         <v>93</v>
       </c>
       <c r="C190" t="n">
-        <v>240250.3987311658</v>
+        <v>260594.7388201463</v>
       </c>
       <c r="D190" t="n">
         <v>2</v>
@@ -9401,7 +9401,7 @@
         <v>94</v>
       </c>
       <c r="C191" t="n">
-        <v>272040.0659987907</v>
+        <v>289470.6744309674</v>
       </c>
       <c r="D191" t="n">
         <v>2</v>

</xml_diff>